<commit_message>
Use MW rather than MW-miles for transmission capacity
</commit_message>
<xml_diff>
--- a/InputData/elec/BTC/BAU Transmission Capacity.xlsx
+++ b/InputData/elec/BTC/BAU Transmission Capacity.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="458" windowWidth="28440" windowHeight="16223" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="458" windowWidth="28440" windowHeight="16223"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
     <sheet name="BTC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>BTC BAU Transmission Capacity</t>
   </si>
@@ -195,10 +195,13 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Total Transmission (MW-miles)</t>
-  </si>
-  <si>
     <t>﻿2018</t>
+  </si>
+  <si>
+    <t>BAU Transmission Capacity (MW)</t>
+  </si>
+  <si>
+    <t>Total Transmission Capacity (MW)</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,13 +244,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -272,10 +268,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -296,13 +291,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -663,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -841,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AP61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="AD52" sqref="AD52"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1691,137 +1683,137 @@
       <c r="I51" t="s">
         <v>54</v>
       </c>
-      <c r="J51" s="15">
+      <c r="J51" s="14">
         <f>C54</f>
-        <v>26399760</v>
+        <v>67312.661999999997</v>
       </c>
       <c r="K51" s="4">
         <f>J51+(L51-J51)/2</f>
-        <v>28060860</v>
-      </c>
-      <c r="L51" s="15">
+        <v>68697.657999999996</v>
+      </c>
+      <c r="L51" s="14">
         <f>C55</f>
-        <v>29721960</v>
+        <v>70082.653999999995</v>
       </c>
       <c r="M51" s="4">
         <f>L51+(($Q$51-$L$51)/5)</f>
-        <v>29824734</v>
+        <v>71590.553199999995</v>
       </c>
       <c r="N51" s="4">
         <f t="shared" ref="N51:P51" si="1">M51+(($Q$51-$L$51)/5)</f>
-        <v>29927508</v>
+        <v>73098.452399999995</v>
       </c>
       <c r="O51" s="4">
         <f t="shared" si="1"/>
-        <v>30030282</v>
+        <v>74606.351599999995</v>
       </c>
       <c r="P51" s="4">
         <f t="shared" si="1"/>
-        <v>30133056</v>
-      </c>
-      <c r="Q51" s="15">
+        <v>76114.250799999994</v>
+      </c>
+      <c r="Q51" s="14">
         <f>C56</f>
-        <v>30235830</v>
+        <v>77622.149999999994</v>
       </c>
       <c r="R51" s="4">
         <f>Q51+(($V$51-$Q$51)/5)</f>
-        <v>30328652</v>
+        <v>78738.6872</v>
       </c>
       <c r="S51" s="4">
         <f t="shared" ref="S51:U51" si="2">R51+(($V$51-$Q$51)/5)</f>
-        <v>30421474</v>
+        <v>79855.224400000006</v>
       </c>
       <c r="T51" s="4">
         <f t="shared" si="2"/>
-        <v>30514296</v>
+        <v>80971.761600000013</v>
       </c>
       <c r="U51" s="4">
         <f t="shared" si="2"/>
-        <v>30607118</v>
-      </c>
-      <c r="V51" s="15">
+        <v>82088.298800000019</v>
+      </c>
+      <c r="V51" s="14">
         <f>C57</f>
-        <v>30699940</v>
+        <v>83204.835999999996</v>
       </c>
       <c r="W51" s="4">
         <f>V51+(($AA$51-$V$51)/5)</f>
-        <v>32626898</v>
+        <v>86073.9568</v>
       </c>
       <c r="X51" s="4">
         <f t="shared" ref="X51:Z51" si="3">W51+(($AA$51-$V$51)/5)</f>
-        <v>34553856</v>
+        <v>88943.077600000004</v>
       </c>
       <c r="Y51" s="4">
         <f t="shared" si="3"/>
-        <v>36480814</v>
+        <v>91812.198400000008</v>
       </c>
       <c r="Z51" s="4">
         <f t="shared" si="3"/>
-        <v>38407772</v>
-      </c>
-      <c r="AA51" s="15">
+        <v>94681.319200000013</v>
+      </c>
+      <c r="AA51" s="14">
         <f>C58</f>
-        <v>40334730</v>
+        <v>97550.44</v>
       </c>
       <c r="AB51" s="4">
         <f>AA51+(($AF$51-$AA$51)/5)</f>
-        <v>40525552</v>
+        <v>99546.486799999999</v>
       </c>
       <c r="AC51" s="4">
         <f t="shared" ref="AC51:AE51" si="4">AB51+(($AF$51-$AA$51)/5)</f>
-        <v>40716374</v>
+        <v>101542.5336</v>
       </c>
       <c r="AD51" s="4">
         <f>AC51+(($AF$51-$AA$51)/5)</f>
-        <v>40907196</v>
+        <v>103538.58039999999</v>
       </c>
       <c r="AE51" s="4">
         <f t="shared" si="4"/>
-        <v>41098018</v>
-      </c>
-      <c r="AF51" s="15">
+        <v>105534.62719999999</v>
+      </c>
+      <c r="AF51" s="14">
         <f>C59</f>
-        <v>41288840</v>
+        <v>107530.674</v>
       </c>
       <c r="AG51" s="4">
         <f>AF51+(($AK$51-$AF$51)/5)</f>
-        <v>42005992</v>
+        <v>110451.6096</v>
       </c>
       <c r="AH51" s="4">
         <f t="shared" ref="AH51:AJ51" si="5">AG51+(($AK$51-$AF$51)/5)</f>
-        <v>42723144</v>
+        <v>113372.54519999999</v>
       </c>
       <c r="AI51" s="4">
         <f t="shared" si="5"/>
-        <v>43440296</v>
+        <v>116293.48079999999</v>
       </c>
       <c r="AJ51" s="4">
         <f t="shared" si="5"/>
-        <v>44157448</v>
-      </c>
-      <c r="AK51" s="15">
+        <v>119214.41639999999</v>
+      </c>
+      <c r="AK51" s="14">
         <f>C60</f>
-        <v>44874600</v>
+        <v>122135.352</v>
       </c>
       <c r="AL51" s="4">
         <f>AK51+(($AP$51-$AK$51)/5)</f>
-        <v>45456812</v>
+        <v>126066.4584</v>
       </c>
       <c r="AM51" s="4">
         <f t="shared" ref="AM51:AO51" si="6">AL51+(($AP$51-$AK$51)/5)</f>
-        <v>46039024</v>
+        <v>129997.56480000001</v>
       </c>
       <c r="AN51" s="4">
         <f t="shared" si="6"/>
-        <v>46621236</v>
+        <v>133928.67120000001</v>
       </c>
       <c r="AO51" s="4">
         <f t="shared" si="6"/>
-        <v>47203448</v>
-      </c>
-      <c r="AP51" s="15">
+        <v>137859.7776</v>
+      </c>
+      <c r="AP51" s="14">
         <f>C61</f>
-        <v>47785660</v>
+        <v>141790.88399999999</v>
       </c>
     </row>
     <row r="53" spans="2:42" x14ac:dyDescent="0.45">
@@ -1829,71 +1821,71 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B54" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C54" s="14">
-        <v>26399760</v>
+        <v>57</v>
+      </c>
+      <c r="C54" s="15">
+        <v>67312.661999999997</v>
       </c>
     </row>
     <row r="55" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B55" s="13">
         <v>2020</v>
       </c>
-      <c r="C55" s="14">
-        <v>29721960</v>
+      <c r="C55" s="15">
+        <v>70082.653999999995</v>
       </c>
     </row>
     <row r="56" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B56" s="13">
         <v>2025</v>
       </c>
-      <c r="C56" s="14">
-        <v>30235830</v>
+      <c r="C56" s="15">
+        <v>77622.149999999994</v>
       </c>
     </row>
     <row r="57" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B57" s="13">
         <v>2030</v>
       </c>
-      <c r="C57" s="14">
-        <v>30699940</v>
+      <c r="C57" s="15">
+        <v>83204.835999999996</v>
       </c>
     </row>
     <row r="58" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B58" s="13">
         <v>2035</v>
       </c>
-      <c r="C58" s="14">
-        <v>40334730</v>
+      <c r="C58" s="15">
+        <v>97550.44</v>
       </c>
     </row>
     <row r="59" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B59" s="13">
         <v>2040</v>
       </c>
-      <c r="C59" s="14">
-        <v>41288840</v>
+      <c r="C59" s="15">
+        <v>107530.674</v>
       </c>
     </row>
     <row r="60" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B60" s="13">
         <v>2045</v>
       </c>
-      <c r="C60" s="14">
-        <v>44874600</v>
+      <c r="C60" s="15">
+        <v>122135.352</v>
       </c>
     </row>
     <row r="61" spans="2:42" x14ac:dyDescent="0.45">
       <c r="B61" s="13">
         <v>2050</v>
       </c>
-      <c r="C61" s="14">
-        <v>47785660</v>
+      <c r="C61" s="15">
+        <v>141790.88399999999</v>
       </c>
     </row>
   </sheetData>
@@ -1914,310 +1906,247 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="42" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="33" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="B1">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C1">
-        <v>2011</v>
+        <v>2020</v>
       </c>
       <c r="D1">
-        <v>2012</v>
+        <v>2021</v>
       </c>
       <c r="E1">
-        <v>2013</v>
+        <v>2022</v>
       </c>
       <c r="F1">
-        <v>2014</v>
+        <v>2023</v>
       </c>
       <c r="G1">
-        <v>2015</v>
+        <v>2024</v>
       </c>
       <c r="H1">
-        <v>2016</v>
+        <v>2025</v>
       </c>
       <c r="I1">
-        <v>2017</v>
+        <v>2026</v>
       </c>
       <c r="J1">
-        <v>2018</v>
+        <v>2027</v>
       </c>
       <c r="K1">
-        <v>2019</v>
+        <v>2028</v>
       </c>
       <c r="L1">
-        <v>2020</v>
+        <v>2029</v>
       </c>
       <c r="M1">
-        <v>2021</v>
+        <v>2030</v>
       </c>
       <c r="N1">
-        <v>2022</v>
+        <v>2031</v>
       </c>
       <c r="O1">
-        <v>2023</v>
+        <v>2032</v>
       </c>
       <c r="P1">
-        <v>2024</v>
+        <v>2033</v>
       </c>
       <c r="Q1">
-        <v>2025</v>
+        <v>2034</v>
       </c>
       <c r="R1">
-        <v>2026</v>
+        <v>2035</v>
       </c>
       <c r="S1">
-        <v>2027</v>
+        <v>2036</v>
       </c>
       <c r="T1">
-        <v>2028</v>
+        <v>2037</v>
       </c>
       <c r="U1">
-        <v>2029</v>
+        <v>2038</v>
       </c>
       <c r="V1">
-        <v>2030</v>
+        <v>2039</v>
       </c>
       <c r="W1">
-        <v>2031</v>
+        <v>2040</v>
       </c>
       <c r="X1">
-        <v>2032</v>
+        <v>2041</v>
       </c>
       <c r="Y1">
-        <v>2033</v>
+        <v>2042</v>
       </c>
       <c r="Z1">
-        <v>2034</v>
+        <v>2043</v>
       </c>
       <c r="AA1">
-        <v>2035</v>
+        <v>2044</v>
       </c>
       <c r="AB1">
-        <v>2036</v>
+        <v>2045</v>
       </c>
       <c r="AC1">
-        <v>2037</v>
+        <v>2046</v>
       </c>
       <c r="AD1">
-        <v>2038</v>
+        <v>2047</v>
       </c>
       <c r="AE1">
-        <v>2039</v>
+        <v>2048</v>
       </c>
       <c r="AF1">
-        <v>2040</v>
+        <v>2049</v>
       </c>
       <c r="AG1">
-        <v>2041</v>
-      </c>
-      <c r="AH1">
-        <v>2042</v>
-      </c>
-      <c r="AI1">
-        <v>2043</v>
-      </c>
-      <c r="AJ1">
-        <v>2044</v>
-      </c>
-      <c r="AK1">
-        <v>2045</v>
-      </c>
-      <c r="AL1">
-        <v>2046</v>
-      </c>
-      <c r="AM1">
-        <v>2047</v>
-      </c>
-      <c r="AN1">
-        <v>2048</v>
-      </c>
-      <c r="AO1">
-        <v>2049</v>
-      </c>
-      <c r="AP1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B2" s="5">
-        <f>'Texas Notes'!B47</f>
-        <v>14498591.87233866</v>
+        <f>'Texas Notes'!J51</f>
+        <v>67312.661999999997</v>
       </c>
       <c r="C2" s="5">
-        <f>'Texas Notes'!C47</f>
-        <v>14509609.039414905</v>
+        <f>'Texas Notes'!K51</f>
+        <v>68697.657999999996</v>
       </c>
       <c r="D2" s="5">
-        <f>'Texas Notes'!D47</f>
-        <v>14520626.20649115</v>
+        <f>'Texas Notes'!L51</f>
+        <v>70082.653999999995</v>
       </c>
       <c r="E2" s="5">
-        <f>'Texas Notes'!E47</f>
-        <v>14531643.373567397</v>
+        <f>'Texas Notes'!M51</f>
+        <v>71590.553199999995</v>
       </c>
       <c r="F2" s="5">
-        <f>'Texas Notes'!F47</f>
-        <v>14542660.540643642</v>
+        <f>'Texas Notes'!N51</f>
+        <v>73098.452399999995</v>
       </c>
       <c r="G2" s="5">
-        <f>'Texas Notes'!G47</f>
-        <v>14553677.707719887</v>
+        <f>'Texas Notes'!O51</f>
+        <v>74606.351599999995</v>
       </c>
       <c r="H2" s="5">
-        <f>'Texas Notes'!H47</f>
-        <v>14564694.874796133</v>
+        <f>'Texas Notes'!P51</f>
+        <v>76114.250799999994</v>
       </c>
       <c r="I2" s="5">
-        <f>'Texas Notes'!I47</f>
-        <v>14575712.041872378</v>
+        <f>'Texas Notes'!Q51</f>
+        <v>77622.149999999994</v>
       </c>
       <c r="J2" s="5">
-        <f>'Texas Notes'!J51</f>
-        <v>26399760</v>
+        <f>'Texas Notes'!R51</f>
+        <v>78738.6872</v>
       </c>
       <c r="K2" s="5">
-        <f>'Texas Notes'!K51</f>
-        <v>28060860</v>
+        <f>'Texas Notes'!S51</f>
+        <v>79855.224400000006</v>
       </c>
       <c r="L2" s="5">
-        <f>'Texas Notes'!L51</f>
-        <v>29721960</v>
+        <f>'Texas Notes'!T51</f>
+        <v>80971.761600000013</v>
       </c>
       <c r="M2" s="5">
-        <f>'Texas Notes'!M51</f>
-        <v>29824734</v>
+        <f>'Texas Notes'!U51</f>
+        <v>82088.298800000019</v>
       </c>
       <c r="N2" s="5">
-        <f>'Texas Notes'!N51</f>
-        <v>29927508</v>
+        <f>'Texas Notes'!V51</f>
+        <v>83204.835999999996</v>
       </c>
       <c r="O2" s="5">
-        <f>'Texas Notes'!O51</f>
-        <v>30030282</v>
+        <f>'Texas Notes'!W51</f>
+        <v>86073.9568</v>
       </c>
       <c r="P2" s="5">
-        <f>'Texas Notes'!P51</f>
-        <v>30133056</v>
+        <f>'Texas Notes'!X51</f>
+        <v>88943.077600000004</v>
       </c>
       <c r="Q2" s="5">
-        <f>'Texas Notes'!Q51</f>
-        <v>30235830</v>
+        <f>'Texas Notes'!Y51</f>
+        <v>91812.198400000008</v>
       </c>
       <c r="R2" s="5">
-        <f>'Texas Notes'!R51</f>
-        <v>30328652</v>
+        <f>'Texas Notes'!Z51</f>
+        <v>94681.319200000013</v>
       </c>
       <c r="S2" s="5">
-        <f>'Texas Notes'!S51</f>
-        <v>30421474</v>
+        <f>'Texas Notes'!AA51</f>
+        <v>97550.44</v>
       </c>
       <c r="T2" s="5">
-        <f>'Texas Notes'!T51</f>
-        <v>30514296</v>
+        <f>'Texas Notes'!AB51</f>
+        <v>99546.486799999999</v>
       </c>
       <c r="U2" s="5">
-        <f>'Texas Notes'!U51</f>
-        <v>30607118</v>
+        <f>'Texas Notes'!AC51</f>
+        <v>101542.5336</v>
       </c>
       <c r="V2" s="5">
-        <f>'Texas Notes'!V51</f>
-        <v>30699940</v>
+        <f>'Texas Notes'!AD51</f>
+        <v>103538.58039999999</v>
       </c>
       <c r="W2" s="5">
-        <f>'Texas Notes'!W51</f>
-        <v>32626898</v>
+        <f>'Texas Notes'!AE51</f>
+        <v>105534.62719999999</v>
       </c>
       <c r="X2" s="5">
-        <f>'Texas Notes'!X51</f>
-        <v>34553856</v>
+        <f>'Texas Notes'!AF51</f>
+        <v>107530.674</v>
       </c>
       <c r="Y2" s="5">
-        <f>'Texas Notes'!Y51</f>
-        <v>36480814</v>
+        <f>'Texas Notes'!AG51</f>
+        <v>110451.6096</v>
       </c>
       <c r="Z2" s="5">
-        <f>'Texas Notes'!Z51</f>
-        <v>38407772</v>
+        <f>'Texas Notes'!AH51</f>
+        <v>113372.54519999999</v>
       </c>
       <c r="AA2" s="5">
-        <f>'Texas Notes'!AA51</f>
-        <v>40334730</v>
+        <f>'Texas Notes'!AI51</f>
+        <v>116293.48079999999</v>
       </c>
       <c r="AB2" s="5">
-        <f>'Texas Notes'!AB51</f>
-        <v>40525552</v>
+        <f>'Texas Notes'!AJ51</f>
+        <v>119214.41639999999</v>
       </c>
       <c r="AC2" s="5">
-        <f>'Texas Notes'!AC51</f>
-        <v>40716374</v>
+        <f>'Texas Notes'!AK51</f>
+        <v>122135.352</v>
       </c>
       <c r="AD2" s="5">
-        <f>'Texas Notes'!AD51</f>
-        <v>40907196</v>
+        <f>'Texas Notes'!AL51</f>
+        <v>126066.4584</v>
       </c>
       <c r="AE2" s="5">
-        <f>'Texas Notes'!AE51</f>
-        <v>41098018</v>
+        <f>'Texas Notes'!AM51</f>
+        <v>129997.56480000001</v>
       </c>
       <c r="AF2" s="5">
-        <f>'Texas Notes'!AF51</f>
-        <v>41288840</v>
+        <f>'Texas Notes'!AN51</f>
+        <v>133928.67120000001</v>
       </c>
       <c r="AG2" s="5">
-        <f>'Texas Notes'!AG51</f>
-        <v>42005992</v>
-      </c>
-      <c r="AH2" s="5">
-        <f>'Texas Notes'!AH51</f>
-        <v>42723144</v>
-      </c>
-      <c r="AI2" s="5">
-        <f>'Texas Notes'!AI51</f>
-        <v>43440296</v>
-      </c>
-      <c r="AJ2" s="5">
-        <f>'Texas Notes'!AJ51</f>
-        <v>44157448</v>
-      </c>
-      <c r="AK2" s="5">
-        <f>'Texas Notes'!AK51</f>
-        <v>44874600</v>
-      </c>
-      <c r="AL2" s="5">
-        <f>'Texas Notes'!AL51</f>
-        <v>45456812</v>
-      </c>
-      <c r="AM2" s="5">
-        <f>'Texas Notes'!AM51</f>
-        <v>46039024</v>
-      </c>
-      <c r="AN2" s="5">
-        <f>'Texas Notes'!AN51</f>
-        <v>46621236</v>
-      </c>
-      <c r="AO2" s="5">
         <f>'Texas Notes'!AO51</f>
-        <v>47203448</v>
-      </c>
-      <c r="AP2" s="5">
-        <f>'Texas Notes'!AP51</f>
-        <v>47785660</v>
+        <v>137859.7776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Smooth DR and transmission additions
</commit_message>
<xml_diff>
--- a/InputData/elec/BTC/BAU Transmission Capacity.xlsx
+++ b/InputData/elec/BTC/BAU Transmission Capacity.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>BTC BAU Transmission Capacity</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>﻿2018</t>
   </si>
   <si>
     <t>BAU Transmission Capacity (MW)</t>
@@ -288,11 +285,11 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -309,6 +306,937 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="#,##0.00000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Texas Notes'!$E$54:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Texas Notes'!$F$54:$F$61</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>67312.661999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70082.653999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77622.149999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83204.835999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97550.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107530.674</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>122135.352</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>141790.88399999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D9C-4AC2-95AC-85DD89E88AC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="394878552"/>
+        <c:axId val="394879536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="394878552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="394879536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="394879536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="394878552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,6 +1289,41 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>383380</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>135731</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>173830</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>164306</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -831,23 +1794,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AP61"/>
+  <dimension ref="A3:AP65"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51:AP51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.86328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1683,210 +2646,234 @@
       <c r="I51" t="s">
         <v>54</v>
       </c>
-      <c r="J51" s="14">
-        <f>C54</f>
+      <c r="J51" s="13">
+        <f>43.73154*J45^2-175624.65332*J45+176389533.8805</f>
+        <v>67983.379700005054</v>
+      </c>
+      <c r="K51" s="13">
+        <f t="shared" ref="K51:AP51" si="1">43.73154*K45^2-175624.65332*K45+176389533.8805</f>
+        <v>68902.953359991312</v>
+      </c>
+      <c r="L51" s="13">
+        <f t="shared" si="1"/>
+        <v>69909.990099966526</v>
+      </c>
+      <c r="M51" s="13">
+        <f t="shared" si="1"/>
+        <v>71004.489919960499</v>
+      </c>
+      <c r="N51" s="13">
+        <f t="shared" si="1"/>
+        <v>72186.452820003033</v>
+      </c>
+      <c r="O51" s="13">
+        <f t="shared" si="1"/>
+        <v>73455.878799974918</v>
+      </c>
+      <c r="P51" s="13">
+        <f t="shared" si="1"/>
+        <v>74812.767859965563</v>
+      </c>
+      <c r="Q51" s="13">
+        <f t="shared" si="1"/>
+        <v>76257.119999945164</v>
+      </c>
+      <c r="R51" s="13">
+        <f t="shared" si="1"/>
+        <v>77788.935220003128</v>
+      </c>
+      <c r="S51" s="13">
+        <f t="shared" si="1"/>
+        <v>79408.213519990444</v>
+      </c>
+      <c r="T51" s="13">
+        <f t="shared" si="1"/>
+        <v>81114.954899966717</v>
+      </c>
+      <c r="U51" s="13">
+        <f t="shared" si="1"/>
+        <v>82909.159359961748</v>
+      </c>
+      <c r="V51" s="13">
+        <f t="shared" si="1"/>
+        <v>84790.826900005341</v>
+      </c>
+      <c r="W51" s="13">
+        <f t="shared" si="1"/>
+        <v>86759.957519978285</v>
+      </c>
+      <c r="X51" s="13">
+        <f t="shared" si="1"/>
+        <v>88816.551219969988</v>
+      </c>
+      <c r="Y51" s="13">
+        <f t="shared" si="1"/>
+        <v>90960.607999950647</v>
+      </c>
+      <c r="Z51" s="13">
+        <f t="shared" si="1"/>
+        <v>93192.12786000967</v>
+      </c>
+      <c r="AA51" s="13">
+        <f t="shared" si="1"/>
+        <v>95511.110799998045</v>
+      </c>
+      <c r="AB51" s="13">
+        <f t="shared" si="1"/>
+        <v>97917.556819975376</v>
+      </c>
+      <c r="AC51" s="13">
+        <f t="shared" si="1"/>
+        <v>100411.46591994166</v>
+      </c>
+      <c r="AD51" s="13">
+        <f t="shared" si="1"/>
+        <v>102992.83809998631</v>
+      </c>
+      <c r="AE51" s="13">
+        <f t="shared" si="1"/>
+        <v>105661.67335999012</v>
+      </c>
+      <c r="AF51" s="13">
+        <f t="shared" si="1"/>
+        <v>108417.97169998288</v>
+      </c>
+      <c r="AG51" s="13">
+        <f t="shared" si="1"/>
+        <v>111261.7331199646</v>
+      </c>
+      <c r="AH51" s="13">
+        <f t="shared" si="1"/>
+        <v>114192.95761999488</v>
+      </c>
+      <c r="AI51" s="13">
+        <f t="shared" si="1"/>
+        <v>117211.64519998431</v>
+      </c>
+      <c r="AJ51" s="13">
+        <f t="shared" si="1"/>
+        <v>120317.7958599627</v>
+      </c>
+      <c r="AK51" s="13">
+        <f t="shared" si="1"/>
+        <v>123511.40959995985</v>
+      </c>
+      <c r="AL51" s="13">
+        <f t="shared" si="1"/>
+        <v>126792.48642000556</v>
+      </c>
+      <c r="AM51" s="13">
+        <f t="shared" si="1"/>
+        <v>130161.02631998062</v>
+      </c>
+      <c r="AN51" s="13">
+        <f t="shared" si="1"/>
+        <v>133617.02929997444</v>
+      </c>
+      <c r="AO51" s="13">
+        <f t="shared" si="1"/>
+        <v>137160.49535995722</v>
+      </c>
+      <c r="AP51" s="13">
+        <f t="shared" si="1"/>
+        <v>140791.42449995875</v>
+      </c>
+    </row>
+    <row r="53" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="E53" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B54" s="15"/>
+      <c r="C54" s="14"/>
+      <c r="E54">
+        <v>2018</v>
+      </c>
+      <c r="F54" s="14">
         <v>67312.661999999997</v>
       </c>
-      <c r="K51" s="4">
-        <f>J51+(L51-J51)/2</f>
-        <v>68697.657999999996</v>
-      </c>
-      <c r="L51" s="14">
-        <f>C55</f>
+    </row>
+    <row r="55" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B55" s="15"/>
+      <c r="C55" s="14"/>
+      <c r="E55">
+        <v>2020</v>
+      </c>
+      <c r="F55" s="14">
         <v>70082.653999999995</v>
       </c>
-      <c r="M51" s="4">
-        <f>L51+(($Q$51-$L$51)/5)</f>
-        <v>71590.553199999995</v>
-      </c>
-      <c r="N51" s="4">
-        <f t="shared" ref="N51:P51" si="1">M51+(($Q$51-$L$51)/5)</f>
-        <v>73098.452399999995</v>
-      </c>
-      <c r="O51" s="4">
-        <f t="shared" si="1"/>
-        <v>74606.351599999995</v>
-      </c>
-      <c r="P51" s="4">
-        <f t="shared" si="1"/>
-        <v>76114.250799999994</v>
-      </c>
-      <c r="Q51" s="14">
-        <f>C56</f>
+    </row>
+    <row r="56" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B56" s="15"/>
+      <c r="C56" s="14"/>
+      <c r="E56">
+        <v>2025</v>
+      </c>
+      <c r="F56" s="14">
         <v>77622.149999999994</v>
       </c>
-      <c r="R51" s="4">
-        <f>Q51+(($V$51-$Q$51)/5)</f>
-        <v>78738.6872</v>
-      </c>
-      <c r="S51" s="4">
-        <f t="shared" ref="S51:U51" si="2">R51+(($V$51-$Q$51)/5)</f>
-        <v>79855.224400000006</v>
-      </c>
-      <c r="T51" s="4">
-        <f t="shared" si="2"/>
-        <v>80971.761600000013</v>
-      </c>
-      <c r="U51" s="4">
-        <f t="shared" si="2"/>
-        <v>82088.298800000019</v>
-      </c>
-      <c r="V51" s="14">
-        <f>C57</f>
+    </row>
+    <row r="57" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B57" s="15"/>
+      <c r="C57" s="14"/>
+      <c r="E57">
+        <v>2030</v>
+      </c>
+      <c r="F57" s="14">
         <v>83204.835999999996</v>
       </c>
-      <c r="W51" s="4">
-        <f>V51+(($AA$51-$V$51)/5)</f>
-        <v>86073.9568</v>
-      </c>
-      <c r="X51" s="4">
-        <f t="shared" ref="X51:Z51" si="3">W51+(($AA$51-$V$51)/5)</f>
-        <v>88943.077600000004</v>
-      </c>
-      <c r="Y51" s="4">
-        <f t="shared" si="3"/>
-        <v>91812.198400000008</v>
-      </c>
-      <c r="Z51" s="4">
-        <f t="shared" si="3"/>
-        <v>94681.319200000013</v>
-      </c>
-      <c r="AA51" s="14">
-        <f>C58</f>
+    </row>
+    <row r="58" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B58" s="15"/>
+      <c r="C58" s="14"/>
+      <c r="E58">
+        <v>2035</v>
+      </c>
+      <c r="F58" s="14">
         <v>97550.44</v>
       </c>
-      <c r="AB51" s="4">
-        <f>AA51+(($AF$51-$AA$51)/5)</f>
-        <v>99546.486799999999</v>
-      </c>
-      <c r="AC51" s="4">
-        <f t="shared" ref="AC51:AE51" si="4">AB51+(($AF$51-$AA$51)/5)</f>
-        <v>101542.5336</v>
-      </c>
-      <c r="AD51" s="4">
-        <f>AC51+(($AF$51-$AA$51)/5)</f>
-        <v>103538.58039999999</v>
-      </c>
-      <c r="AE51" s="4">
-        <f t="shared" si="4"/>
-        <v>105534.62719999999</v>
-      </c>
-      <c r="AF51" s="14">
-        <f>C59</f>
+    </row>
+    <row r="59" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B59" s="15"/>
+      <c r="C59" s="14"/>
+      <c r="E59">
+        <v>2040</v>
+      </c>
+      <c r="F59" s="14">
         <v>107530.674</v>
       </c>
-      <c r="AG51" s="4">
-        <f>AF51+(($AK$51-$AF$51)/5)</f>
-        <v>110451.6096</v>
-      </c>
-      <c r="AH51" s="4">
-        <f t="shared" ref="AH51:AJ51" si="5">AG51+(($AK$51-$AF$51)/5)</f>
-        <v>113372.54519999999</v>
-      </c>
-      <c r="AI51" s="4">
-        <f t="shared" si="5"/>
-        <v>116293.48079999999</v>
-      </c>
-      <c r="AJ51" s="4">
-        <f t="shared" si="5"/>
-        <v>119214.41639999999</v>
-      </c>
-      <c r="AK51" s="14">
-        <f>C60</f>
+    </row>
+    <row r="60" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B60" s="15"/>
+      <c r="C60" s="14"/>
+      <c r="E60">
+        <v>2045</v>
+      </c>
+      <c r="F60" s="14">
         <v>122135.352</v>
       </c>
-      <c r="AL51" s="4">
-        <f>AK51+(($AP$51-$AK$51)/5)</f>
-        <v>126066.4584</v>
-      </c>
-      <c r="AM51" s="4">
-        <f t="shared" ref="AM51:AO51" si="6">AL51+(($AP$51-$AK$51)/5)</f>
-        <v>129997.56480000001</v>
-      </c>
-      <c r="AN51" s="4">
-        <f t="shared" si="6"/>
-        <v>133928.67120000001</v>
-      </c>
-      <c r="AO51" s="4">
-        <f t="shared" si="6"/>
-        <v>137859.7776</v>
-      </c>
-      <c r="AP51" s="14">
-        <f>C61</f>
+    </row>
+    <row r="61" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B61" s="15"/>
+      <c r="C61" s="14"/>
+      <c r="E61">
+        <v>2050</v>
+      </c>
+      <c r="F61" s="14">
         <v>141790.88399999999</v>
       </c>
     </row>
-    <row r="53" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B54" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="15">
-        <v>67312.661999999997</v>
-      </c>
-    </row>
-    <row r="55" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B55" s="13">
-        <v>2020</v>
-      </c>
-      <c r="C55" s="15">
-        <v>70082.653999999995</v>
-      </c>
-    </row>
-    <row r="56" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B56" s="13">
-        <v>2025</v>
-      </c>
-      <c r="C56" s="15">
-        <v>77622.149999999994</v>
-      </c>
-    </row>
-    <row r="57" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B57" s="13">
-        <v>2030</v>
-      </c>
-      <c r="C57" s="15">
-        <v>83204.835999999996</v>
-      </c>
-    </row>
-    <row r="58" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B58" s="13">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="15">
-        <v>97550.44</v>
-      </c>
-    </row>
-    <row r="59" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B59" s="13">
-        <v>2040</v>
-      </c>
-      <c r="C59" s="15">
-        <v>107530.674</v>
-      </c>
-    </row>
-    <row r="60" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B60" s="13">
-        <v>2045</v>
-      </c>
-      <c r="C60" s="15">
-        <v>122135.352</v>
-      </c>
-    </row>
-    <row r="61" spans="2:42" x14ac:dyDescent="0.45">
-      <c r="B61" s="13">
-        <v>2050</v>
-      </c>
-      <c r="C61" s="15">
-        <v>141790.88399999999</v>
-      </c>
+    <row r="64" spans="2:42" x14ac:dyDescent="0.45">
+      <c r="B64" s="15"/>
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" s="15"/>
+      <c r="C65" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1897,7 +2884,8 @@
     <hyperlink ref="B23" r:id="rId5" display="https://www.nerc.com/pa/RAPA/ra/Reliability Assessments DL/NERC_LTRA_2018_12202018.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1909,7 +2897,7 @@
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2:AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2018,135 +3006,135 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5">
-        <f>'Texas Notes'!J51</f>
-        <v>67312.661999999997</v>
+        <f>'Texas Notes'!K51</f>
+        <v>68902.953359991312</v>
       </c>
       <c r="C2" s="5">
-        <f>'Texas Notes'!K51</f>
-        <v>68697.657999999996</v>
+        <f>'Texas Notes'!L51</f>
+        <v>69909.990099966526</v>
       </c>
       <c r="D2" s="5">
-        <f>'Texas Notes'!L51</f>
-        <v>70082.653999999995</v>
+        <f>'Texas Notes'!M51</f>
+        <v>71004.489919960499</v>
       </c>
       <c r="E2" s="5">
-        <f>'Texas Notes'!M51</f>
-        <v>71590.553199999995</v>
+        <f>'Texas Notes'!N51</f>
+        <v>72186.452820003033</v>
       </c>
       <c r="F2" s="5">
-        <f>'Texas Notes'!N51</f>
-        <v>73098.452399999995</v>
+        <f>'Texas Notes'!O51</f>
+        <v>73455.878799974918</v>
       </c>
       <c r="G2" s="5">
-        <f>'Texas Notes'!O51</f>
-        <v>74606.351599999995</v>
+        <f>'Texas Notes'!P51</f>
+        <v>74812.767859965563</v>
       </c>
       <c r="H2" s="5">
-        <f>'Texas Notes'!P51</f>
-        <v>76114.250799999994</v>
+        <f>'Texas Notes'!Q51</f>
+        <v>76257.119999945164</v>
       </c>
       <c r="I2" s="5">
-        <f>'Texas Notes'!Q51</f>
-        <v>77622.149999999994</v>
+        <f>'Texas Notes'!R51</f>
+        <v>77788.935220003128</v>
       </c>
       <c r="J2" s="5">
-        <f>'Texas Notes'!R51</f>
-        <v>78738.6872</v>
+        <f>'Texas Notes'!S51</f>
+        <v>79408.213519990444</v>
       </c>
       <c r="K2" s="5">
-        <f>'Texas Notes'!S51</f>
-        <v>79855.224400000006</v>
+        <f>'Texas Notes'!T51</f>
+        <v>81114.954899966717</v>
       </c>
       <c r="L2" s="5">
-        <f>'Texas Notes'!T51</f>
-        <v>80971.761600000013</v>
+        <f>'Texas Notes'!U51</f>
+        <v>82909.159359961748</v>
       </c>
       <c r="M2" s="5">
-        <f>'Texas Notes'!U51</f>
-        <v>82088.298800000019</v>
+        <f>'Texas Notes'!V51</f>
+        <v>84790.826900005341</v>
       </c>
       <c r="N2" s="5">
-        <f>'Texas Notes'!V51</f>
-        <v>83204.835999999996</v>
+        <f>'Texas Notes'!W51</f>
+        <v>86759.957519978285</v>
       </c>
       <c r="O2" s="5">
-        <f>'Texas Notes'!W51</f>
-        <v>86073.9568</v>
+        <f>'Texas Notes'!X51</f>
+        <v>88816.551219969988</v>
       </c>
       <c r="P2" s="5">
-        <f>'Texas Notes'!X51</f>
-        <v>88943.077600000004</v>
+        <f>'Texas Notes'!Y51</f>
+        <v>90960.607999950647</v>
       </c>
       <c r="Q2" s="5">
-        <f>'Texas Notes'!Y51</f>
-        <v>91812.198400000008</v>
+        <f>'Texas Notes'!Z51</f>
+        <v>93192.12786000967</v>
       </c>
       <c r="R2" s="5">
-        <f>'Texas Notes'!Z51</f>
-        <v>94681.319200000013</v>
+        <f>'Texas Notes'!AA51</f>
+        <v>95511.110799998045</v>
       </c>
       <c r="S2" s="5">
-        <f>'Texas Notes'!AA51</f>
-        <v>97550.44</v>
+        <f>'Texas Notes'!AB51</f>
+        <v>97917.556819975376</v>
       </c>
       <c r="T2" s="5">
-        <f>'Texas Notes'!AB51</f>
-        <v>99546.486799999999</v>
+        <f>'Texas Notes'!AC51</f>
+        <v>100411.46591994166</v>
       </c>
       <c r="U2" s="5">
-        <f>'Texas Notes'!AC51</f>
-        <v>101542.5336</v>
+        <f>'Texas Notes'!AD51</f>
+        <v>102992.83809998631</v>
       </c>
       <c r="V2" s="5">
-        <f>'Texas Notes'!AD51</f>
-        <v>103538.58039999999</v>
+        <f>'Texas Notes'!AE51</f>
+        <v>105661.67335999012</v>
       </c>
       <c r="W2" s="5">
-        <f>'Texas Notes'!AE51</f>
-        <v>105534.62719999999</v>
+        <f>'Texas Notes'!AF51</f>
+        <v>108417.97169998288</v>
       </c>
       <c r="X2" s="5">
-        <f>'Texas Notes'!AF51</f>
-        <v>107530.674</v>
+        <f>'Texas Notes'!AG51</f>
+        <v>111261.7331199646</v>
       </c>
       <c r="Y2" s="5">
-        <f>'Texas Notes'!AG51</f>
-        <v>110451.6096</v>
+        <f>'Texas Notes'!AH51</f>
+        <v>114192.95761999488</v>
       </c>
       <c r="Z2" s="5">
-        <f>'Texas Notes'!AH51</f>
-        <v>113372.54519999999</v>
+        <f>'Texas Notes'!AI51</f>
+        <v>117211.64519998431</v>
       </c>
       <c r="AA2" s="5">
-        <f>'Texas Notes'!AI51</f>
-        <v>116293.48079999999</v>
+        <f>'Texas Notes'!AJ51</f>
+        <v>120317.7958599627</v>
       </c>
       <c r="AB2" s="5">
-        <f>'Texas Notes'!AJ51</f>
-        <v>119214.41639999999</v>
+        <f>'Texas Notes'!AK51</f>
+        <v>123511.40959995985</v>
       </c>
       <c r="AC2" s="5">
-        <f>'Texas Notes'!AK51</f>
-        <v>122135.352</v>
+        <f>'Texas Notes'!AL51</f>
+        <v>126792.48642000556</v>
       </c>
       <c r="AD2" s="5">
-        <f>'Texas Notes'!AL51</f>
-        <v>126066.4584</v>
+        <f>'Texas Notes'!AM51</f>
+        <v>130161.02631998062</v>
       </c>
       <c r="AE2" s="5">
-        <f>'Texas Notes'!AM51</f>
-        <v>129997.56480000001</v>
+        <f>'Texas Notes'!AN51</f>
+        <v>133617.02929997444</v>
       </c>
       <c r="AF2" s="5">
-        <f>'Texas Notes'!AN51</f>
-        <v>133928.67120000001</v>
+        <f>'Texas Notes'!AO51</f>
+        <v>137160.49535995722</v>
       </c>
       <c r="AG2" s="5">
-        <f>'Texas Notes'!AO51</f>
-        <v>137859.7776</v>
+        <f>'Texas Notes'!AP51</f>
+        <v>140791.42449995875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>